<commit_message>
Tela pro conselho implementada, correcao de bugs
</commit_message>
<xml_diff>
--- a/others/projeto_cep.xlsx
+++ b/others/projeto_cep.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>Alterações realizadas, conforme solicitação</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Validação para não permitir valor maior que o bimestre</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
     <t>Validar para não permitir curso e disciplina com mesmo nome</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Talvez trocar o js que abre as paginas dos links da tela de turma do menu boletim, por ancora</t>
+  </si>
+  <si>
+    <t>Colocar colunas de exame e status na tela de boletim do aluno</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,18 +206,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -234,6 +242,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,10 +540,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -544,31 +556,31 @@
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
+      <c r="F3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -576,7 +588,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -584,7 +596,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -592,110 +604,115 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>9</v>
+      <c r="A8" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
+      <c r="A9" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>23</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="B19" s="3"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
alteracao na planilha de atividades do projeto
</commit_message>
<xml_diff>
--- a/others/projeto_cep.xlsx
+++ b/others/projeto_cep.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Alterações realizadas, conforme solicitação</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Colocar colunas de exame e status na tela de boletim do aluno</t>
+  </si>
+  <si>
+    <t>Arrumar o layout da tela de detalhes da turma</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -204,17 +207,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -245,7 +237,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,6 +705,13 @@
       <c r="A25" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
bug fixed (2), alerta de erro na rede ao alterar notas, classificacao da turma e aluno por ano letivo
</commit_message>
<xml_diff>
--- a/others/projeto_cep.xlsx
+++ b/others/projeto_cep.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Alterações realizadas, conforme solicitação</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Arrumar o layout da tela de detalhes da turma</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -238,6 +241,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,10 +538,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -548,11 +554,11 @@
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -615,103 +621,111 @@
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="10" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="10"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="10"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="10" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="10"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="10"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="3"/>
+      <c r="B25" s="10"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>